<commit_message>
Remove sort of grapes if not vine
</commit_message>
<xml_diff>
--- a/wine2.xlsx
+++ b/wine2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Илья\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PyProjects\DevManLessons\vine_site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1B18A6-D0D5-46C6-8795-EDD6EAD4D101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F235889F-B473-441E-AB5D-AB7789484EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Название</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>konyak_kizilovyi.png</t>
+  </si>
+  <si>
+    <t>Закуски</t>
+  </si>
+  <si>
+    <t>Рыба</t>
+  </si>
+  <si>
+    <t>Мясо</t>
+  </si>
+  <si>
+    <t>Сыр</t>
   </si>
 </sst>
 </file>
@@ -396,10 +408,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -575,6 +587,39 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3">
+        <v>40000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>